<commit_message>
Adiciona relatório e coentários
</commit_message>
<xml_diff>
--- a/TrabalhoParte2/Resultados/Resultado das Compressões.xlsx
+++ b/TrabalhoParte2/Resultados/Resultado das Compressões.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\UFJF\Disciplinas\4° Período\Estrutura de Dados II\Trabalho\TrabalhoParte2\Resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE9DF3B-29A8-42AF-A12C-674D700499C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BE42F1-8980-4A69-AA58-F23EC3F6E447}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1CC7ADB8-F0F4-4DCD-99B6-5D226C9EC457}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{1CC7ADB8-F0F4-4DCD-99B6-5D226C9EC457}"/>
   </bookViews>
   <sheets>
     <sheet name="Seed1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="8">
   <si>
     <t xml:space="preserve">                                           Tempo de Compressão                                  </t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Chave(Sinopse)</t>
+  </si>
+  <si>
+    <t>Tamanho real</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -153,6 +156,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -168,6 +173,3697 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Tempo de Compressão</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Média!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LZW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Média!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Média!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.4352399999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24447619999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2171939999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5050300000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.713000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ACB5-4317-9F5B-EAF41FF07419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Média!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Huffman</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Média!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Média!$B$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.8057999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8732400000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29600019999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49650660000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9488180000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ACB5-4317-9F5B-EAF41FF07419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="80"/>
+        <c:overlap val="25"/>
+        <c:axId val="684344479"/>
+        <c:axId val="550199663"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="684344479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Número de sinopses</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="550199663"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="550199663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tempo em s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="684344479"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light (Títulos)"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" b="0" cap="none" baseline="0">
+                <a:latin typeface="Calibri Light (Títulos)"/>
+              </a:rPr>
+              <a:t>Tamanho do Arquivo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri Light (Títulos)"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Média!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Chave(Sinopse)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Média!$B$8:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Média!$B$9:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.0372800009776133E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31411773693059536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5821584370266157</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1344798811000345</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.111422847438901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A1F-4903-A153-BC0BDDFD2E01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Média!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LZW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Média!$B$8:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Média!$B$10:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.6127275796222241E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32147083377088076</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4758604370819564</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.833279114285935</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.800233409073998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0A1F-4903-A153-BC0BDDFD2E01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Média!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Huffman</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Média!$B$8:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Média!$B$11:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.7534030923187258E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18390142198172751</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92852682869833403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8388572177495579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2881881554380072</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0A1F-4903-A153-BC0BDDFD2E01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="442331999"/>
+        <c:axId val="387289599"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="442331999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Número de Sinopses</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="387289599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="387289599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tamanho em mb</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="442331999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600">
+                <a:latin typeface="Calibri Light (Títulos)"/>
+              </a:rPr>
+              <a:t>Taxa de Compressão</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Média!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LZW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Média!$B$15:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Média!$B$16:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.1897490303159945</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0234050523770779</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93281844427838256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90390761502605965</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83621853987712069</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4F47-4187-9F62-FBD42688DA88}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Média!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Huffman</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Média!$B$15:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Média!$B$17:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5771808178157104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58543885769867621</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58686752711429879</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58665280544666998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.58733894129905129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4F47-4187-9F62-FBD42688DA88}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="682317407"/>
+        <c:axId val="493062351"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Média!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tamanho real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Média!$B$15:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Média!$B$18:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4F47-4187-9F62-FBD42688DA88}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="682317407"/>
+        <c:axId val="493062351"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="682317407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="900" cap="all" baseline="0"/>
+                  <a:t>Número de Sinopses</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493062351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="493062351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="900" cap="all" baseline="0"/>
+                  <a:t>% em relação ao tamanho real</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="682317407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D29851C-8A14-4428-A5B9-C3172D3E3958}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{758753F0-B58A-4C28-9F2F-E76A91EE86B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4167811A-2C57-43E7-A8F1-70CF91003A57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -733,8 +4429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDAC3074-E89F-4858-89E8-4DAD030A4103}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,8 +4551,12 @@
       <c r="D9" s="3">
         <v>1575936</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="6">
+        <v>3151278</v>
+      </c>
+      <c r="F9" s="6">
+        <v>14111237</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -871,8 +4571,12 @@
       <c r="D10" s="3">
         <v>1471342</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="6">
+        <v>2848205</v>
+      </c>
+      <c r="F10" s="6">
+        <v>11800078</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -891,8 +4595,8 @@
         <v>924350</v>
       </c>
       <c r="E11" s="3">
-        <f>QUOTIENT(14624328,8)</f>
-        <v>1828041</v>
+        <f>QUOTIENT(14803560,8)</f>
+        <v>1850445</v>
       </c>
       <c r="F11" s="3">
         <f>QUOTIENT(66304634,8)</f>
@@ -945,13 +4649,13 @@
         <f t="shared" si="0"/>
         <v>0.93363055352501623</v>
       </c>
-      <c r="E16" s="3" t="e">
+      <c r="E16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="3" t="e">
+        <v>0.90382536862822005</v>
+      </c>
+      <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.83621853987712058</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,13 +4674,13 @@
         <f t="shared" si="1"/>
         <v>0.58654031635802473</v>
       </c>
-      <c r="E17" s="3" t="e">
+      <c r="E17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="3" t="e">
+        <v>0.58720461983995065</v>
+      </c>
+      <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.58733894129905129</v>
       </c>
     </row>
   </sheetData>
@@ -989,7 +4693,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,21 +4735,41 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="B3" s="4">
+        <v>2.7959999999999999E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.23969499999999999</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.2702800000000001</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.6085500000000001</v>
+      </c>
+      <c r="F3" s="4">
+        <v>11.576499999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="B4" s="4">
+        <v>3.9960000000000004E-3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3.9933000000000003E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.35954799999999998</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.46737499999999998</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2.82823</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1081,41 +4805,61 @@
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="3">
+        <v>29394</v>
+      </c>
+      <c r="C9" s="3">
+        <v>306925</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1575846</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3146955</v>
+      </c>
+      <c r="F9" s="6">
+        <v>14111237</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="B10" s="3">
+        <v>35204</v>
+      </c>
+      <c r="C10" s="3">
+        <v>313910</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1470383</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2843697</v>
+      </c>
+      <c r="F10" s="6">
+        <v>11800078</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3">
-        <f>QUOTIENT(128407,8)</f>
-        <v>16050</v>
+        <f>QUOTIENT(136921,8)</f>
+        <v>17115</v>
       </c>
       <c r="C11" s="3">
-        <f>QUOTIENT(1488194,8)</f>
-        <v>186024</v>
+        <f>QUOTIENT(1431072,8)</f>
+        <v>178884</v>
       </c>
       <c r="D11" s="3">
-        <f>QUOTIENT(7452566,8)</f>
-        <v>931570</v>
+        <f>QUOTIENT(7394709,8)</f>
+        <v>924338</v>
       </c>
       <c r="E11" s="3">
-        <f>QUOTIENT(14624328,8)</f>
-        <v>1828041</v>
+        <f>QUOTIENT(14783335,8)</f>
+        <v>1847916</v>
       </c>
       <c r="F11" s="3">
         <f>QUOTIENT(66304634,8)</f>
@@ -1156,50 +4900,50 @@
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="3" t="e">
+      <c r="B16" s="3">
         <f>B10/B9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" s="3" t="e">
+        <v>1.1976593862693066</v>
+      </c>
+      <c r="C16" s="3">
         <f t="shared" ref="C16:F16" si="0">C10/C9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D16" s="3" t="e">
+        <v>1.0227580027694063</v>
+      </c>
+      <c r="D16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E16" s="3" t="e">
+        <v>0.93307531319684789</v>
+      </c>
+      <c r="E16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="3" t="e">
+        <v>0.9036344656977936</v>
+      </c>
+      <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.83621853987712058</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="3" t="e">
+      <c r="B17" s="3">
         <f>B11/B9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="3" t="e">
+        <v>0.58226168605837925</v>
+      </c>
+      <c r="C17" s="3">
         <f t="shared" ref="C17:F17" si="1">C11/C9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="3" t="e">
+        <v>0.58282642339333712</v>
+      </c>
+      <c r="D17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="3" t="e">
+        <v>0.58656619999670023</v>
+      </c>
+      <c r="E17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="3" t="e">
+        <v>0.58720763404624465</v>
+      </c>
+      <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.58733894129905129</v>
       </c>
     </row>
   </sheetData>
@@ -1212,7 +4956,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" activeCellId="1" sqref="B3:F4 B9:F10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,21 +4998,41 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="B3" s="4">
+        <v>3.1955999999999998E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.21171799999999999</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.1505000000000001</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.3489</v>
+      </c>
+      <c r="F3" s="4">
+        <v>11.7845</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="B4" s="4">
+        <v>3.9960000000000004E-3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4.7935999999999999E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.29557499999999998</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.45935700000000002</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3.0679099999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1304,41 +5068,61 @@
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="3">
+        <v>32472</v>
+      </c>
+      <c r="C9" s="3">
+        <v>313573</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1599098</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3123076</v>
+      </c>
+      <c r="F9" s="6">
+        <v>14111237</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="B10" s="3">
+        <v>38349</v>
+      </c>
+      <c r="C10" s="3">
+        <v>321123</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1490251</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2822806</v>
+      </c>
+      <c r="F10" s="6">
+        <v>11800078</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3">
-        <f>QUOTIENT(128407,8)</f>
-        <v>16050</v>
+        <f>QUOTIENT(150122,8)</f>
+        <v>18765</v>
       </c>
       <c r="C11" s="3">
-        <f>QUOTIENT(1488194,8)</f>
-        <v>186024</v>
+        <f>QUOTIENT(1469451,8)</f>
+        <v>183681</v>
       </c>
       <c r="D11" s="3">
-        <f>QUOTIENT(7452566,8)</f>
-        <v>931570</v>
+        <f>QUOTIENT(7530312,8)</f>
+        <v>941289</v>
       </c>
       <c r="E11" s="3">
-        <f>QUOTIENT(14624328,8)</f>
-        <v>1828041</v>
+        <f>QUOTIENT(14652829,8)</f>
+        <v>1831603</v>
       </c>
       <c r="F11" s="3">
         <f>QUOTIENT(66304634,8)</f>
@@ -1379,50 +5163,50 @@
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="3" t="e">
+      <c r="B16" s="3">
         <f>B10/B9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" s="3" t="e">
+        <v>1.1809866962305986</v>
+      </c>
+      <c r="C16" s="3">
         <f t="shared" ref="C16:F16" si="0">C10/C9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D16" s="3" t="e">
+        <v>1.0240773280862829</v>
+      </c>
+      <c r="D16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E16" s="3" t="e">
+        <v>0.93193225180695616</v>
+      </c>
+      <c r="E16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="3" t="e">
+        <v>0.90385440508011972</v>
+      </c>
+      <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.83621853987712058</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="3" t="e">
+      <c r="B17" s="3">
         <f>B11/B9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="3" t="e">
+        <v>0.57788248337028825</v>
+      </c>
+      <c r="C17" s="3">
         <f t="shared" ref="C17:F17" si="1">C11/C9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="3" t="e">
+        <v>0.58576790731344852</v>
+      </c>
+      <c r="D17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="3" t="e">
+        <v>0.58863746937335926</v>
+      </c>
+      <c r="E17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="3" t="e">
+        <v>0.58647404033715478</v>
+      </c>
+      <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.58733894129905129</v>
       </c>
     </row>
   </sheetData>
@@ -1435,7 +5219,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" activeCellId="1" sqref="B3:F4 B9:F10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,21 +5261,41 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="B3" s="4">
+        <v>4.3937999999999998E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.31957000000000002</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.2403900000000001</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.4624799999999998</v>
+      </c>
+      <c r="F3" s="4">
+        <v>11.299200000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="B4" s="4">
+        <v>8.0199999999999994E-3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5.1930999999999998E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.285603</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.45730100000000001</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2.91988</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1527,41 +5331,61 @@
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="3">
+        <v>29931</v>
+      </c>
+      <c r="C9" s="3">
+        <v>316986</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1572973</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3131273</v>
+      </c>
+      <c r="F9" s="6">
+        <v>14111237</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="B10" s="3">
+        <v>35581</v>
+      </c>
+      <c r="C10" s="3">
+        <v>324005</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1468221</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2831633</v>
+      </c>
+      <c r="F10" s="6">
+        <v>11800078</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3">
-        <f>QUOTIENT(128407,8)</f>
-        <v>16050</v>
+        <f>QUOTIENT(137179,8)</f>
+        <v>17147</v>
       </c>
       <c r="C11" s="3">
-        <f>QUOTIENT(1488194,8)</f>
-        <v>186024</v>
+        <f>QUOTIENT(1486148,8)</f>
+        <v>185768</v>
       </c>
       <c r="D11" s="3">
-        <f>QUOTIENT(7452566,8)</f>
-        <v>931570</v>
+        <f>QUOTIENT(7368209,8)</f>
+        <v>921026</v>
       </c>
       <c r="E11" s="3">
-        <f>QUOTIENT(14624328,8)</f>
-        <v>1828041</v>
+        <f>QUOTIENT(14689282,8)</f>
+        <v>1836160</v>
       </c>
       <c r="F11" s="3">
         <f>QUOTIENT(66304634,8)</f>
@@ -1602,50 +5426,50 @@
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="3" t="e">
+      <c r="B16" s="3">
         <f>B10/B9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" s="3" t="e">
+        <v>1.1887674985800676</v>
+      </c>
+      <c r="C16" s="3">
         <f t="shared" ref="C16:F16" si="0">C10/C9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D16" s="3" t="e">
+        <v>1.0221429337573269</v>
+      </c>
+      <c r="D16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E16" s="3" t="e">
+        <v>0.93340508705489544</v>
+      </c>
+      <c r="E16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="3" t="e">
+        <v>0.90430728971890983</v>
+      </c>
+      <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.83621853987712058</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="3" t="e">
+      <c r="B17" s="3">
         <f>B11/B9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="3" t="e">
+        <v>0.57288430055794992</v>
+      </c>
+      <c r="C17" s="3">
         <f t="shared" ref="C17:F17" si="1">C11/C9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="3" t="e">
+        <v>0.58604480954994853</v>
+      </c>
+      <c r="D17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="3" t="e">
+        <v>0.58553198306646081</v>
+      </c>
+      <c r="E17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="3" t="e">
+        <v>0.58639409594755876</v>
+      </c>
+      <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.58733894129905129</v>
       </c>
     </row>
   </sheetData>
@@ -1655,10 +5479,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3637B8A1-0CAC-4185-AFA8-28B7BAA141EF}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,22 +5501,20 @@
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="7">
         <v>100</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="7">
         <v>1000</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="7">
         <v>5000</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="7">
         <v>10000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="7">
         <v>45573</v>
       </c>
     </row>
@@ -1702,23 +5524,23 @@
       </c>
       <c r="B3" s="4">
         <f>(Seed1!B3+Seed2!B3+Seed3!B3+Seed4!B3+Seed5!B3)/5</f>
-        <v>1.3581599999999999E-2</v>
+        <v>3.4352399999999998E-2</v>
       </c>
       <c r="C3" s="4">
         <f>(Seed1!C3+Seed2!C3+Seed3!C3+Seed4!C3+Seed5!C3)/5</f>
-        <v>9.0279599999999988E-2</v>
+        <v>0.24447619999999998</v>
       </c>
       <c r="D3" s="4">
         <f>(Seed1!D3+Seed2!D3+Seed3!D3+Seed4!D3+Seed5!D3)/5</f>
-        <v>0.48496000000000006</v>
+        <v>1.2171939999999999</v>
       </c>
       <c r="E3" s="4">
         <f>(Seed1!E3+Seed2!E3+Seed3!E3+Seed4!E3+Seed5!E3)/5</f>
-        <v>1.0210440000000001</v>
+        <v>2.5050300000000001</v>
       </c>
       <c r="F3" s="4">
         <f>(Seed1!F3+Seed2!F3+Seed3!F3+Seed4!F3+Seed5!F3)/5</f>
-        <v>4.7809600000000003</v>
+        <v>11.713000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,23 +5549,23 @@
       </c>
       <c r="B4" s="4">
         <f>(Seed1!B4+Seed2!B4+Seed3!B4+Seed4!B4+Seed5!B4)/5</f>
-        <v>1.6034000000000001E-3</v>
+        <v>4.8057999999999998E-3</v>
       </c>
       <c r="C4" s="4">
         <f>(Seed1!C4+Seed2!C4+Seed3!C4+Seed4!C4+Seed5!C4)/5</f>
-        <v>2.07724E-2</v>
+        <v>4.8732400000000002E-2</v>
       </c>
       <c r="D4" s="4">
         <f>(Seed1!D4+Seed2!D4+Seed3!D4+Seed4!D4+Seed5!D4)/5</f>
-        <v>0.10785499999999999</v>
+        <v>0.29600019999999999</v>
       </c>
       <c r="E4" s="4">
         <f>(Seed1!E4+Seed2!E4+Seed3!E4+Seed4!E4+Seed5!E4)/5</f>
-        <v>0.21970000000000001</v>
+        <v>0.49650660000000002</v>
       </c>
       <c r="F4" s="4">
         <f>(Seed1!F4+Seed2!F4+Seed3!F4+Seed4!F4+Seed5!F4)/5</f>
-        <v>1.1856139999999999</v>
+        <v>2.9488180000000002</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,22 +5579,20 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="7">
         <v>100</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="7">
         <v>1000</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="7">
         <v>5000</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="7">
         <v>10000</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="7">
         <v>45573</v>
       </c>
     </row>
@@ -1781,24 +5601,24 @@
         <v>6</v>
       </c>
       <c r="B9" s="4">
-        <f>(Seed1!B9+Seed2!B9+Seed3!B9+Seed4!B9+Seed5!B9)/5</f>
-        <v>12013</v>
+        <f>((Seed1!B9+Seed2!B9+Seed3!B9+Seed4!B9+Seed5!B9)/5)/999986.83</f>
+        <v>3.0372800009776133E-2</v>
       </c>
       <c r="C9" s="4">
-        <f>(Seed1!C9+Seed2!C9+Seed3!C9+Seed4!C9+Seed5!C9)/5</f>
-        <v>126616.8</v>
+        <f>((Seed1!C9+Seed2!C9+Seed3!C9+Seed4!C9+Seed5!C9)/5)/999986.83</f>
+        <v>0.31411773693059536</v>
       </c>
       <c r="D9" s="4">
-        <f>(Seed1!D9+Seed2!D9+Seed3!D9+Seed4!D9+Seed5!D9)/5</f>
-        <v>632554.19999999995</v>
+        <f>((Seed1!D9+Seed2!D9+Seed3!D9+Seed4!D9+Seed5!D9)/5)/999986.83</f>
+        <v>1.5821584370266157</v>
       </c>
       <c r="E9" s="4">
-        <f>(Seed1!E9+Seed2!E9+Seed3!E9+Seed4!E9+Seed5!E9)/5</f>
-        <v>623922.19999999995</v>
+        <f>((Seed1!E9+Seed2!E9+Seed3!E9+Seed4!E9+Seed5!E9)/5)/999986.83</f>
+        <v>3.1344798811000345</v>
       </c>
       <c r="F9" s="4">
-        <f>(Seed1!F9+Seed2!F9+Seed3!F9+Seed4!F9+Seed5!F9)/5</f>
-        <v>2822247.4</v>
+        <f>((Seed1!F9+Seed2!F9+Seed3!F9+Seed4!F9+Seed5!F9)/5)/999986.83</f>
+        <v>14.111422847438901</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1806,24 +5626,24 @@
         <v>5</v>
       </c>
       <c r="B10" s="4">
-        <f>(Seed1!B10+Seed2!B10+Seed3!B10+Seed4!B10+Seed5!B10)/5</f>
-        <v>14300</v>
+        <f>((Seed1!B10+Seed2!B10+Seed3!B10+Seed4!B10+Seed5!B10)/5)/999986.83</f>
+        <v>3.6127275796222241E-2</v>
       </c>
       <c r="C10" s="4">
-        <f>(Seed1!C10+Seed2!C10+Seed3!C10+Seed4!C10+Seed5!C10)/5</f>
-        <v>129659</v>
+        <f>((Seed1!C10+Seed2!C10+Seed3!C10+Seed4!C10+Seed5!C10)/5)/999986.83</f>
+        <v>0.32147083377088076</v>
       </c>
       <c r="D10" s="4">
-        <f>(Seed1!D10+Seed2!D10+Seed3!D10+Seed4!D10+Seed5!D10)/5</f>
-        <v>590070</v>
+        <f>((Seed1!D10+Seed2!D10+Seed3!D10+Seed4!D10+Seed5!D10)/5)/999986.83</f>
+        <v>1.4758604370819564</v>
       </c>
       <c r="E10" s="4">
-        <f>(Seed1!E10+Seed2!E10+Seed3!E10+Seed4!E10+Seed5!E10)/5</f>
-        <v>563973.6</v>
+        <f>((Seed1!E10+Seed2!E10+Seed3!E10+Seed4!E10+Seed5!E10)/5)/999986.83</f>
+        <v>2.833279114285935</v>
       </c>
       <c r="F10" s="4">
-        <f>(Seed1!F10+Seed2!F10+Seed3!F10+Seed4!F10+Seed5!F10)/5</f>
-        <v>2360015.6</v>
+        <f>((Seed1!F10+Seed2!F10+Seed3!F10+Seed4!F10+Seed5!F10)/5)/999986.83</f>
+        <v>11.800233409073998</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1831,24 +5651,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="4">
-        <f>(Seed1!B11+Seed2!B11+Seed3!B11+Seed4!B11+Seed5!B11)/5</f>
-        <v>16558.400000000001</v>
+        <f>((Seed1!B11+Seed2!B11+Seed3!B11+Seed4!B11+Seed5!B11)/5)/999986.83</f>
+        <v>1.7534030923187258E-2</v>
       </c>
       <c r="C11" s="4">
-        <f>(Seed1!C11+Seed2!C11+Seed3!C11+Seed4!C11+Seed5!C11)/5</f>
-        <v>185846.8</v>
+        <f>((Seed1!C11+Seed2!C11+Seed3!C11+Seed4!C11+Seed5!C11)/5)/999986.83</f>
+        <v>0.18390142198172751</v>
       </c>
       <c r="D11" s="4">
-        <f>(Seed1!D11+Seed2!D11+Seed3!D11+Seed4!D11+Seed5!D11)/5</f>
-        <v>930126</v>
+        <f>((Seed1!D11+Seed2!D11+Seed3!D11+Seed4!D11+Seed5!D11)/5)/999986.83</f>
+        <v>0.92852682869833403</v>
       </c>
       <c r="E11" s="4">
-        <f>(Seed1!E11+Seed2!E11+Seed3!E11+Seed4!E11+Seed5!E11)/5</f>
-        <v>1828041</v>
+        <f>((Seed1!E11+Seed2!E11+Seed3!E11+Seed4!E11+Seed5!E11)/5)/999986.83</f>
+        <v>1.8388572177495579</v>
       </c>
       <c r="F11" s="4">
-        <f>(Seed1!F11+Seed2!F11+Seed3!F11+Seed4!F11+Seed5!F11)/5</f>
-        <v>8288079</v>
+        <f>((Seed1!F11+Seed2!F11+Seed3!F11+Seed4!F11+Seed5!F11)/5)/999986.83</f>
+        <v>8.2881881554380072</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1862,22 +5682,20 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="7">
         <v>100</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="7">
         <v>1000</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="7">
         <v>5000</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="7">
         <v>10000</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="7">
         <v>45573</v>
       </c>
     </row>
@@ -1885,53 +5703,74 @@
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="e">
+      <c r="B16" s="4">
         <f>(Seed1!B16+Seed2!B16+Seed3!B16+Seed4!B16+Seed5!B16)/5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" s="4" t="e">
+        <v>1.1897490303159945</v>
+      </c>
+      <c r="C16" s="4">
         <f>(Seed1!C16+Seed2!C16+Seed3!C16+Seed4!C16+Seed5!C16)/5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D16" s="4" t="e">
+        <v>1.0234050523770779</v>
+      </c>
+      <c r="D16" s="4">
         <f>(Seed1!D16+Seed2!D16+Seed3!D16+Seed4!D16+Seed5!D16)/5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E16" s="4" t="e">
+        <v>0.93281844427838256</v>
+      </c>
+      <c r="E16" s="4">
         <f>(Seed1!E16+Seed2!E16+Seed3!E16+Seed4!E16+Seed5!E16)/5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="4" t="e">
+        <v>0.90390761502605965</v>
+      </c>
+      <c r="F16" s="4">
         <f>(Seed1!F16+Seed2!F16+Seed3!F16+Seed4!F16+Seed5!F16)/5</f>
-        <v>#DIV/0!</v>
+        <v>0.83621853987712069</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="4" t="e">
+      <c r="B17" s="4">
         <f>(Seed1!B17+Seed2!B17+Seed3!B17+Seed4!B17+Seed5!B17)/5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="4" t="e">
+        <v>0.5771808178157104</v>
+      </c>
+      <c r="C17" s="4">
         <f>(Seed1!C17+Seed2!C17+Seed3!C17+Seed4!C17+Seed5!C17)/5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="4" t="e">
+        <v>0.58543885769867621</v>
+      </c>
+      <c r="D17" s="4">
         <f>(Seed1!D17+Seed2!D17+Seed3!D17+Seed4!D17+Seed5!D17)/5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="4" t="e">
+        <v>0.58686752711429879</v>
+      </c>
+      <c r="E17" s="4">
         <f>(Seed1!E17+Seed2!E17+Seed3!E17+Seed4!E17+Seed5!E17)/5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="4" t="e">
+        <v>0.58665280544666998</v>
+      </c>
+      <c r="F17" s="4">
         <f>(Seed1!F17+Seed2!F17+Seed3!F17+Seed4!F17+Seed5!F17)/5</f>
-        <v>#DIV/0!</v>
+        <v>0.58733894129905129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>